<commit_message>
Completando TODOs, agregando preview y actualizando README.md
</commit_message>
<xml_diff>
--- a/participantes.xlsx
+++ b/participantes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guido\Documents\GUIDO\practica\React\apps\sorteo-app-00\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,34 +24,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>guido</t>
-  </si>
-  <si>
-    <t>rivoira</t>
-  </si>
-  <si>
-    <t>jose</t>
-  </si>
-  <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>pedro</t>
-  </si>
-  <si>
-    <t>tomas</t>
-  </si>
-  <si>
-    <t>cuki</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>lorem</t>
+  </si>
+  <si>
+    <t>ipsum</t>
+  </si>
+  <si>
+    <t>dolor</t>
+  </si>
+  <si>
+    <t>asit</t>
+  </si>
+  <si>
+    <t>amet</t>
+  </si>
+  <si>
+    <t>joe</t>
+  </si>
+  <si>
+    <t>doe</t>
+  </si>
+  <si>
+    <t>foo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +64,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,9 +99,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,52 +383,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>